<commit_message>
updated Cortana_Recording_Metadata.xlsx and added 231006 pkls
</commit_message>
<xml_diff>
--- a/recording_metadata/Cortana_Recording_Metadata.xlsx
+++ b/recording_metadata/Cortana_Recording_Metadata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="14"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ER" sheetId="1" state="visible" r:id="rId2"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1864" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1866" uniqueCount="626">
   <si>
     <t xml:space="preserve">Round </t>
   </si>
@@ -2506,7 +2506,7 @@
       <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.42"/>
   </cols>
@@ -2779,11 +2779,11 @@
   </sheetPr>
   <dimension ref="A1:Q57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.8046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.32"/>
@@ -3958,10 +3958,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -4031,11 +4031,11 @@
   </sheetPr>
   <dimension ref="A1:H121"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="14.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="22.92"/>
@@ -6580,9 +6580,9 @@
       <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.11"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6630,7 +6630,7 @@
       <selection pane="topLeft" activeCell="C25" activeCellId="0" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.23"/>
@@ -7158,11 +7158,11 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="27.53"/>
@@ -7793,7 +7793,7 @@
       <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
   </cols>
@@ -8040,10 +8040,10 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1" ySplit="0" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topRight" activeCell="B24" activeCellId="0" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="9.59"/>
@@ -9328,7 +9328,7 @@
       </c>
       <c r="F70" s="11"/>
     </row>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="5" t="n">
         <v>45258</v>
       </c>
@@ -9345,7 +9345,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="5" t="n">
         <v>45258</v>
       </c>
@@ -9362,7 +9362,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="5" t="n">
         <v>45258</v>
       </c>
@@ -9379,7 +9379,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="5" t="n">
         <v>45258</v>
       </c>
@@ -9396,7 +9396,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="23" t="n">
         <v>45265</v>
       </c>
@@ -9414,7 +9414,7 @@
       </c>
       <c r="F75" s="25"/>
     </row>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="5" t="n">
         <v>45265</v>
       </c>
@@ -9431,7 +9431,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="5" t="n">
         <v>45265</v>
       </c>
@@ -9448,7 +9448,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="n">
         <v>45265</v>
       </c>
@@ -9466,7 +9466,7 @@
       </c>
       <c r="F78" s="11"/>
     </row>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="5" t="n">
         <v>45267</v>
       </c>
@@ -9483,7 +9483,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="5" t="n">
         <v>45267</v>
       </c>
@@ -9500,7 +9500,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="5" t="n">
         <v>45267</v>
       </c>
@@ -9757,11 +9757,11 @@
   </sheetPr>
   <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.86"/>
@@ -10754,11 +10754,11 @@
   </sheetPr>
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D4" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.42"/>
@@ -11151,7 +11151,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="60" t="n">
         <v>45205</v>
       </c>
@@ -11162,12 +11162,14 @@
         <v>257</v>
       </c>
       <c r="D23" s="59"/>
-      <c r="E23" s="59"/>
+      <c r="E23" s="56" t="s">
+        <v>258</v>
+      </c>
       <c r="F23" s="0" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="61" t="n">
         <v>45205</v>
       </c>
@@ -11178,7 +11180,9 @@
         <v>259</v>
       </c>
       <c r="D24" s="56"/>
-      <c r="E24" s="56"/>
+      <c r="E24" s="56" t="s">
+        <v>260</v>
+      </c>
       <c r="F24" s="0" t="s">
         <v>260</v>
       </c>
@@ -12378,7 +12382,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="5" t="s">
@@ -12974,7 +12978,7 @@
       <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.19"/>
@@ -13651,7 +13655,7 @@
       <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.39"/>
@@ -14667,7 +14671,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.11"/>

</xml_diff>